<commit_message>
Censored data analysis (linear and GLM) + updated plots
</commit_message>
<xml_diff>
--- a/summary_tracking_complete.xlsx
+++ b/summary_tracking_complete.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BI78"/>
+  <dimension ref="A1:BJ78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -672,6 +672,11 @@
           <t>dist_trav_30min_body_out</t>
         </is>
       </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>Visual_exp</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -868,6 +873,9 @@
       <c r="BI2">
         <v>0</v>
       </c>
+      <c r="BJ2">
+        <v>105</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3">
@@ -1064,6 +1072,9 @@
       <c r="BI3">
         <v>0</v>
       </c>
+      <c r="BJ3">
+        <v>0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4">
@@ -1260,6 +1271,9 @@
       <c r="BI4">
         <v>53.959036928</v>
       </c>
+      <c r="BJ4">
+        <v>155</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5">
@@ -1456,6 +1470,9 @@
       <c r="BI5">
         <v>0</v>
       </c>
+      <c r="BJ5">
+        <v>243</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -1652,6 +1669,9 @@
       <c r="BI6">
         <v>0</v>
       </c>
+      <c r="BJ6">
+        <v>155</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7">
@@ -1848,6 +1868,9 @@
       <c r="BI7">
         <v>0</v>
       </c>
+      <c r="BJ7">
+        <v>1108</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8">
@@ -2041,6 +2064,9 @@
       <c r="BI8">
         <v>0</v>
       </c>
+      <c r="BJ8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9">
@@ -2237,6 +2263,9 @@
       <c r="BI9">
         <v>0</v>
       </c>
+      <c r="BJ9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10">
@@ -2433,6 +2462,9 @@
       <c r="BI10">
         <v>134.850822292</v>
       </c>
+      <c r="BJ10">
+        <v>245</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11">
@@ -2629,6 +2661,9 @@
       <c r="BI11">
         <v>0</v>
       </c>
+      <c r="BJ11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12">
@@ -2822,6 +2857,9 @@
       <c r="BI12">
         <v>0</v>
       </c>
+      <c r="BJ12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13">
@@ -3018,6 +3056,9 @@
       <c r="BI13">
         <v>87.1682587289</v>
       </c>
+      <c r="BJ13">
+        <v>140</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14">
@@ -3214,6 +3255,9 @@
       <c r="BI14">
         <v>0</v>
       </c>
+      <c r="BJ14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15">
@@ -3410,6 +3454,9 @@
       <c r="BI15">
         <v>0</v>
       </c>
+      <c r="BJ15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16">
@@ -3606,6 +3653,9 @@
       <c r="BI16">
         <v>0</v>
       </c>
+      <c r="BJ16">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17">
@@ -3802,6 +3852,9 @@
       <c r="BI17">
         <v>94.83043631629999</v>
       </c>
+      <c r="BJ17">
+        <v>110</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18">
@@ -3998,6 +4051,9 @@
       <c r="BI18">
         <v>0</v>
       </c>
+      <c r="BJ18">
+        <v>294</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19">
@@ -4194,6 +4250,9 @@
       <c r="BI19">
         <v>0</v>
       </c>
+      <c r="BJ19">
+        <v>0</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20">
@@ -4390,6 +4449,9 @@
       <c r="BI20">
         <v>0</v>
       </c>
+      <c r="BJ20">
+        <v>123</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21">
@@ -4583,6 +4645,9 @@
       <c r="BI21">
         <v>0</v>
       </c>
+      <c r="BJ21">
+        <v>531</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22">
@@ -4776,6 +4841,9 @@
       <c r="BI22">
         <v>85.755232096</v>
       </c>
+      <c r="BJ22">
+        <v>500</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23">
@@ -4969,6 +5037,9 @@
       <c r="BI23">
         <v>156.0485786097</v>
       </c>
+      <c r="BJ23">
+        <v>485</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24">
@@ -5162,6 +5233,9 @@
       <c r="BI24">
         <v>106.651700849</v>
       </c>
+      <c r="BJ24">
+        <v>237</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25">
@@ -5355,6 +5429,9 @@
       <c r="BI25">
         <v>0</v>
       </c>
+      <c r="BJ25">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26">
@@ -5551,6 +5628,9 @@
       <c r="BI26">
         <v>0</v>
       </c>
+      <c r="BJ26">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27">
@@ -5747,6 +5827,9 @@
       <c r="BI27">
         <v>0</v>
       </c>
+      <c r="BJ27">
+        <v>289</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28">
@@ -5943,6 +6026,9 @@
       <c r="BI28">
         <v>115.689266338</v>
       </c>
+      <c r="BJ28">
+        <v>205</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29">
@@ -6139,6 +6225,9 @@
       <c r="BI29">
         <v>85.9006444444</v>
       </c>
+      <c r="BJ29">
+        <v>253</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30">
@@ -6335,6 +6424,9 @@
       <c r="BI30">
         <v>97.59974628339999</v>
       </c>
+      <c r="BJ30">
+        <v>193</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31">
@@ -6531,6 +6623,9 @@
       <c r="BI31">
         <v>83.6186979527</v>
       </c>
+      <c r="BJ31">
+        <v>359</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32">
@@ -6727,6 +6822,9 @@
       <c r="BI32">
         <v>109.372537696</v>
       </c>
+      <c r="BJ32">
+        <v>407</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33">
@@ -6923,6 +7021,9 @@
       <c r="BI33">
         <v>0</v>
       </c>
+      <c r="BJ33">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34">
@@ -7119,6 +7220,9 @@
       <c r="BI34">
         <v>155.295083402</v>
       </c>
+      <c r="BJ34">
+        <v>743</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35">
@@ -7315,6 +7419,9 @@
       <c r="BI35">
         <v>0</v>
       </c>
+      <c r="BJ35">
+        <v>350</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36">
@@ -7511,6 +7618,9 @@
       <c r="BI36">
         <v>0</v>
       </c>
+      <c r="BJ36">
+        <v>371</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37">
@@ -7707,6 +7817,9 @@
       <c r="BI37">
         <v>0</v>
       </c>
+      <c r="BJ37">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38">
@@ -7903,6 +8016,9 @@
       <c r="BI38">
         <v>130.592298752</v>
       </c>
+      <c r="BJ38">
+        <v>68</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39">
@@ -8099,6 +8215,9 @@
       <c r="BI39">
         <v>127.5684101063</v>
       </c>
+      <c r="BJ39">
+        <v>172</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40">
@@ -8295,6 +8414,9 @@
       <c r="BI40">
         <v>55.375485867</v>
       </c>
+      <c r="BJ40">
+        <v>447</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41">
@@ -8491,6 +8613,9 @@
       <c r="BI41">
         <v>0</v>
       </c>
+      <c r="BJ41">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42">
@@ -8687,6 +8812,9 @@
       <c r="BI42">
         <v>0</v>
       </c>
+      <c r="BJ42">
+        <v>136</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43">
@@ -8883,6 +9011,9 @@
       <c r="BI43">
         <v>0</v>
       </c>
+      <c r="BJ43">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44">
@@ -9079,6 +9210,9 @@
       <c r="BI44">
         <v>103.163733472</v>
       </c>
+      <c r="BJ44">
+        <v>549</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45">
@@ -9275,6 +9409,9 @@
       <c r="BI45">
         <v>73.402168129</v>
       </c>
+      <c r="BJ45">
+        <v>132</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46">
@@ -9471,6 +9608,9 @@
       <c r="BI46">
         <v>80.42873317900001</v>
       </c>
+      <c r="BJ46">
+        <v>106</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47">
@@ -9667,6 +9807,9 @@
       <c r="BI47">
         <v>109.044053422</v>
       </c>
+      <c r="BJ47">
+        <v>191</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48">
@@ -9860,6 +10003,9 @@
       <c r="BI48">
         <v>137.560560446</v>
       </c>
+      <c r="BJ48">
+        <v>211</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49">
@@ -10056,6 +10202,9 @@
       <c r="BI49">
         <v>0</v>
       </c>
+      <c r="BJ49">
+        <v>525</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50">
@@ -10252,6 +10401,9 @@
       <c r="BI50">
         <v>0</v>
       </c>
+      <c r="BJ50">
+        <v>89</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51">
@@ -10445,6 +10597,9 @@
       <c r="BI51">
         <v>0</v>
       </c>
+      <c r="BJ51">
+        <v>571</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52">
@@ -10638,6 +10793,9 @@
       <c r="BI52">
         <v>0</v>
       </c>
+      <c r="BJ52">
+        <v>419</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53">
@@ -10831,6 +10989,9 @@
       <c r="BI53">
         <v>0</v>
       </c>
+      <c r="BJ53">
+        <v>64</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54">
@@ -11024,6 +11185,9 @@
       <c r="BI54">
         <v>128.1463967038</v>
       </c>
+      <c r="BJ54">
+        <v>138</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55">
@@ -11217,6 +11381,9 @@
       <c r="BI55">
         <v>0</v>
       </c>
+      <c r="BJ55">
+        <v>690</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56">
@@ -11410,6 +11577,9 @@
       <c r="BI56">
         <v>151.616284415</v>
       </c>
+      <c r="BJ56">
+        <v>281</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57">
@@ -11603,6 +11773,9 @@
       <c r="BI57">
         <v>0</v>
       </c>
+      <c r="BJ57">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58">
@@ -11796,6 +11969,9 @@
       <c r="BI58">
         <v>0</v>
       </c>
+      <c r="BJ58">
+        <v>177</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59">
@@ -11989,6 +12165,9 @@
       <c r="BI59">
         <v>0</v>
       </c>
+      <c r="BJ59">
+        <v>433</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60">
@@ -12182,6 +12361,9 @@
       <c r="BI60">
         <v>0</v>
       </c>
+      <c r="BJ60">
+        <v>311</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61">
@@ -12378,6 +12560,9 @@
       <c r="BI61">
         <v>0</v>
       </c>
+      <c r="BJ61">
+        <v>511</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62">
@@ -12574,6 +12759,9 @@
       <c r="BI62">
         <v>99.15457831800001</v>
       </c>
+      <c r="BJ62">
+        <v>162</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63">
@@ -12767,6 +12955,9 @@
       <c r="BI63">
         <v>107.9400711688</v>
       </c>
+      <c r="BJ63">
+        <v>572</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64">
@@ -12963,6 +13154,9 @@
       <c r="BI64">
         <v>0</v>
       </c>
+      <c r="BJ64">
+        <v>0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65">
@@ -13159,6 +13353,9 @@
       <c r="BI65">
         <v>93.370780098</v>
       </c>
+      <c r="BJ65">
+        <v>201</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66">
@@ -13355,6 +13552,9 @@
       <c r="BI66">
         <v>0</v>
       </c>
+      <c r="BJ66">
+        <v>656</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67">
@@ -13551,6 +13751,9 @@
       <c r="BI67">
         <v>94.596163937</v>
       </c>
+      <c r="BJ67">
+        <v>221</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68">
@@ -13744,6 +13947,9 @@
       <c r="BI68">
         <v>0</v>
       </c>
+      <c r="BJ68">
+        <v>0</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69">
@@ -13940,6 +14146,9 @@
       <c r="BI69">
         <v>194.844537196</v>
       </c>
+      <c r="BJ69">
+        <v>586</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70">
@@ -14136,6 +14345,9 @@
       <c r="BI70">
         <v>0</v>
       </c>
+      <c r="BJ70">
+        <v>532</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71">
@@ -14329,6 +14541,9 @@
       <c r="BI71">
         <v>141.0301472726</v>
       </c>
+      <c r="BJ71">
+        <v>254</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72">
@@ -14525,6 +14740,9 @@
       <c r="BI72">
         <v>0</v>
       </c>
+      <c r="BJ72">
+        <v>0</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73">
@@ -14721,6 +14939,9 @@
       <c r="BI73">
         <v>0</v>
       </c>
+      <c r="BJ73">
+        <v>884</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74">
@@ -14917,6 +15138,9 @@
       <c r="BI74">
         <v>127.79899625</v>
       </c>
+      <c r="BJ74">
+        <v>256</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75">
@@ -15113,6 +15337,9 @@
       <c r="BI75">
         <v>137.905860639</v>
       </c>
+      <c r="BJ75">
+        <v>255</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76">
@@ -15309,6 +15536,9 @@
       <c r="BI76">
         <v>0</v>
       </c>
+      <c r="BJ76">
+        <v>521</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77">
@@ -15502,6 +15732,9 @@
       <c r="BI77">
         <v>0</v>
       </c>
+      <c r="BJ77">
+        <v>1806</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78">
@@ -15697,6 +15930,9 @@
       </c>
       <c r="BI78">
         <v>158.930296279</v>
+      </c>
+      <c r="BJ78">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>